<commit_message>
Adding repo for Burgess et al. Long-standing historical dynamics suggest a slow-growth, high-inequality economic future.
</commit_message>
<xml_diff>
--- a/Burgess-et-al-fisheries-files/Data-files/GCB-data-and-Schwalm-et-al-2020/Global_Carbon_Budget_2021v0.4.xlsx
+++ b/Burgess-et-al-fisheries-files/Data-files/GCB-data-and-Schwalm-et-al-2020/Global_Carbon_Budget_2021v0.4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mburgess/Desktop/Archives/AR5 paper drafts/ClimateAR5Kaya/Burgess-et-al-fisheries-files/GCB-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mburgess/Desktop/Archives/AR5 paper drafts/ClimateAR5Kaya/Burgess-et-al-fisheries-files/Data-files/GCB-data-and-Schwalm-et-al-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD8AFE5-AF8A-7148-9189-7100190D2BA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A409841-53CD-4A46-BABE-54C0142B0760}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4580" yWindow="460" windowWidth="24220" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3958,8 +3958,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22:L83"/>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23:M83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -4675,6 +4675,10 @@
         <f>I22-J22</f>
         <v>4.6952784695613765</v>
       </c>
+      <c r="M22" s="41">
+        <f>B22+C22</f>
+        <v>4.2626008688212504</v>
+      </c>
       <c r="N22" s="14"/>
       <c r="O22" s="14"/>
       <c r="P22" s="14"/>
@@ -4734,6 +4738,10 @@
         <f t="shared" ref="L23:L83" si="2">I23-J23</f>
         <v>3.9309084162326773</v>
       </c>
+      <c r="M23" s="41">
+        <f t="shared" ref="M23:M83" si="3">B23+C23</f>
+        <v>4.41564760491518</v>
+      </c>
       <c r="N23" s="14"/>
       <c r="O23" s="14"/>
       <c r="P23" s="14"/>
@@ -4793,6 +4801,10 @@
         <f t="shared" si="2"/>
         <v>1.4594761585727998</v>
       </c>
+      <c r="M24" s="41">
+        <f t="shared" si="3"/>
+        <v>4.4323884946897696</v>
+      </c>
       <c r="N24" s="14"/>
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
@@ -4852,6 +4864,10 @@
         <f t="shared" si="2"/>
         <v>4.41937173305669</v>
       </c>
+      <c r="M25" s="41">
+        <f t="shared" si="3"/>
+        <v>4.4516405923999205</v>
+      </c>
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
       <c r="P25" s="14"/>
@@ -4911,6 +4927,10 @@
         <f t="shared" si="2"/>
         <v>3.914866786872091</v>
       </c>
+      <c r="M26" s="41">
+        <f t="shared" si="3"/>
+        <v>4.4552256287126202</v>
+      </c>
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
       <c r="P26" s="14"/>
@@ -4970,6 +4990,10 @@
         <f t="shared" si="2"/>
         <v>3.6419461565660161</v>
       </c>
+      <c r="M27" s="41">
+        <f t="shared" si="3"/>
+        <v>4.5195854407731701</v>
+      </c>
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
       <c r="P27" s="14"/>
@@ -5029,6 +5053,10 @@
         <f t="shared" si="2"/>
         <v>3.1614045825552868</v>
       </c>
+      <c r="M28" s="41">
+        <f t="shared" si="3"/>
+        <v>4.5059370139150099</v>
+      </c>
       <c r="N28" s="14"/>
       <c r="O28" s="14"/>
       <c r="P28" s="14"/>
@@ -5088,6 +5116,10 @@
         <f t="shared" si="2"/>
         <v>3.2549746027160458</v>
       </c>
+      <c r="M29" s="41">
+        <f t="shared" si="3"/>
+        <v>4.5873649697696104</v>
+      </c>
       <c r="N29" s="14"/>
       <c r="O29" s="14"/>
       <c r="P29" s="14"/>
@@ -5147,6 +5179,10 @@
         <f t="shared" si="2"/>
         <v>3.3591715978435759</v>
       </c>
+      <c r="M30" s="41">
+        <f t="shared" si="3"/>
+        <v>4.7136653951376299</v>
+      </c>
       <c r="N30" s="14"/>
       <c r="O30" s="14"/>
       <c r="P30" s="14"/>
@@ -5206,6 +5242,10 @@
         <f t="shared" si="2"/>
         <v>3.1563024239976878</v>
       </c>
+      <c r="M31" s="41">
+        <f t="shared" si="3"/>
+        <v>4.90298005354797</v>
+      </c>
       <c r="N31" s="14"/>
       <c r="O31" s="14"/>
       <c r="P31" s="14"/>
@@ -5265,6 +5305,10 @@
         <f t="shared" si="2"/>
         <v>2.9755810894633408</v>
       </c>
+      <c r="M32" s="41">
+        <f t="shared" si="3"/>
+        <v>5.0496761917548003</v>
+      </c>
       <c r="N32" s="14"/>
       <c r="O32" s="14"/>
       <c r="P32" s="14"/>
@@ -5324,6 +5368,10 @@
         <f t="shared" si="2"/>
         <v>3.29721996951604</v>
       </c>
+      <c r="M33" s="41">
+        <f t="shared" si="3"/>
+        <v>5.3524442302499304</v>
+      </c>
       <c r="N33" s="14"/>
       <c r="O33" s="14"/>
       <c r="P33" s="14"/>
@@ -5383,6 +5431,10 @@
         <f t="shared" si="2"/>
         <v>3.1417492017272801</v>
       </c>
+      <c r="M34" s="41">
+        <f t="shared" si="3"/>
+        <v>5.50301066067024</v>
+      </c>
       <c r="N34" s="14"/>
       <c r="O34" s="14"/>
       <c r="P34" s="14"/>
@@ -5442,6 +5494,10 @@
         <f t="shared" si="2"/>
         <v>3.1206815563614549</v>
       </c>
+      <c r="M35" s="41">
+        <f t="shared" si="3"/>
+        <v>5.7034719470554798</v>
+      </c>
       <c r="N35" s="14"/>
       <c r="O35" s="14"/>
       <c r="P35" s="14"/>
@@ -5501,6 +5557,10 @@
         <f t="shared" si="2"/>
         <v>3.0430054585347124</v>
       </c>
+      <c r="M36" s="41">
+        <f t="shared" si="3"/>
+        <v>5.8998794692637198</v>
+      </c>
       <c r="N36" s="14"/>
       <c r="O36" s="14"/>
       <c r="P36" s="14"/>
@@ -5560,6 +5620,10 @@
         <f t="shared" si="2"/>
         <v>2.3962082823685718</v>
       </c>
+      <c r="M37" s="41">
+        <f t="shared" si="3"/>
+        <v>5.8346223780902999</v>
+      </c>
       <c r="N37" s="14"/>
       <c r="O37" s="14"/>
       <c r="P37" s="14"/>
@@ -5619,6 +5683,10 @@
         <f t="shared" si="2"/>
         <v>3.35249217364656</v>
       </c>
+      <c r="M38" s="41">
+        <f t="shared" si="3"/>
+        <v>6.0694460628311102</v>
+      </c>
       <c r="N38" s="14"/>
       <c r="O38" s="14"/>
       <c r="P38" s="14"/>
@@ -5678,6 +5746,10 @@
         <f t="shared" si="2"/>
         <v>2.6775206484081404</v>
       </c>
+      <c r="M39" s="41">
+        <f t="shared" si="3"/>
+        <v>6.2102175744522405</v>
+      </c>
       <c r="N39" s="14"/>
       <c r="O39" s="14"/>
       <c r="P39" s="14"/>
@@ -5737,6 +5809,10 @@
         <f t="shared" si="2"/>
         <v>2.8775663775356111</v>
       </c>
+      <c r="M40" s="41">
+        <f t="shared" si="3"/>
+        <v>6.31491842830886</v>
+      </c>
       <c r="N40" s="14"/>
       <c r="O40" s="14"/>
       <c r="P40" s="14"/>
@@ -5796,6 +5872,10 @@
         <f t="shared" si="2"/>
         <v>2.6581732155844042</v>
       </c>
+      <c r="M41" s="41">
+        <f t="shared" si="3"/>
+        <v>6.3580400039154998</v>
+      </c>
       <c r="N41" s="14"/>
       <c r="O41" s="14"/>
       <c r="P41" s="14"/>
@@ -5855,6 +5935,10 @@
         <f t="shared" si="2"/>
         <v>2.526038073445549</v>
       </c>
+      <c r="M42" s="41">
+        <f t="shared" si="3"/>
+        <v>6.5128208372355498</v>
+      </c>
       <c r="N42" s="14"/>
       <c r="O42" s="14"/>
       <c r="P42" s="14"/>
@@ -5914,6 +5998,10 @@
         <f t="shared" si="2"/>
         <v>2.5355699852899503</v>
       </c>
+      <c r="M43" s="41">
+        <f t="shared" si="3"/>
+        <v>6.4510097708044203</v>
+      </c>
       <c r="N43" s="14"/>
       <c r="O43" s="14"/>
       <c r="P43" s="14"/>
@@ -5973,6 +6061,10 @@
         <f t="shared" si="2"/>
         <v>2.7173230721907489</v>
       </c>
+      <c r="M44" s="41">
+        <f t="shared" si="3"/>
+        <v>6.3705803983990297</v>
+      </c>
       <c r="N44" s="14"/>
       <c r="O44" s="14"/>
       <c r="P44" s="14"/>
@@ -6032,6 +6124,10 @@
         <f t="shared" si="2"/>
         <v>2.5205709074751264</v>
       </c>
+      <c r="M45" s="41">
+        <f t="shared" si="3"/>
+        <v>6.3071631186388801</v>
+      </c>
       <c r="N45" s="14"/>
       <c r="O45" s="14"/>
       <c r="P45" s="14"/>
@@ -6091,6 +6187,10 @@
         <f t="shared" si="2"/>
         <v>2.682195654847348</v>
       </c>
+      <c r="M46" s="41">
+        <f t="shared" si="3"/>
+        <v>6.4572110307464996</v>
+      </c>
       <c r="N46" s="14"/>
       <c r="O46" s="14"/>
       <c r="P46" s="14"/>
@@ -6150,6 +6250,10 @@
         <f t="shared" si="2"/>
         <v>3.1638806350417723</v>
       </c>
+      <c r="M47" s="41">
+        <f t="shared" si="3"/>
+        <v>6.7766359003536598</v>
+      </c>
       <c r="N47" s="14"/>
       <c r="O47" s="14"/>
       <c r="P47" s="14"/>
@@ -6209,6 +6313,10 @@
         <f t="shared" si="2"/>
         <v>2.7496929245684543</v>
       </c>
+      <c r="M48" s="41">
+        <f t="shared" si="3"/>
+        <v>6.8828779585849098</v>
+      </c>
       <c r="N48" s="14"/>
       <c r="O48" s="14"/>
       <c r="P48" s="14"/>
@@ -6268,6 +6376,10 @@
         <f t="shared" si="2"/>
         <v>2.9415357766512109</v>
       </c>
+      <c r="M49" s="41">
+        <f t="shared" si="3"/>
+        <v>6.9453731953963693</v>
+      </c>
       <c r="N49" s="14"/>
       <c r="O49" s="14"/>
       <c r="P49" s="14"/>
@@ -6327,6 +6439,10 @@
         <f t="shared" si="2"/>
         <v>2.8541895689581311</v>
       </c>
+      <c r="M50" s="41">
+        <f t="shared" si="3"/>
+        <v>7.0677580601030208</v>
+      </c>
       <c r="N50" s="14"/>
       <c r="O50" s="14"/>
       <c r="P50" s="14"/>
@@ -6386,6 +6502,10 @@
         <f t="shared" si="2"/>
         <v>2.4809909182084366</v>
       </c>
+      <c r="M51" s="41">
+        <f t="shared" si="3"/>
+        <v>7.2612985865520496</v>
+      </c>
       <c r="N51" s="14"/>
       <c r="O51" s="14"/>
       <c r="P51" s="14"/>
@@ -6445,6 +6565,10 @@
         <f t="shared" si="2"/>
         <v>2.0901666924412088</v>
       </c>
+      <c r="M52" s="41">
+        <f t="shared" si="3"/>
+        <v>7.3036428877910105</v>
+      </c>
       <c r="N52" s="14"/>
       <c r="O52" s="14"/>
       <c r="P52" s="14"/>
@@ -6504,6 +6628,10 @@
         <f t="shared" si="2"/>
         <v>2.3339462851249113</v>
       </c>
+      <c r="M53" s="41">
+        <f t="shared" si="3"/>
+        <v>7.3823013799125006</v>
+      </c>
       <c r="N53" s="14"/>
       <c r="O53" s="14"/>
       <c r="P53" s="14"/>
@@ -6563,6 +6691,10 @@
         <f t="shared" si="2"/>
         <v>2.2784463332591929</v>
       </c>
+      <c r="M54" s="41">
+        <f t="shared" si="3"/>
+        <v>7.4918635422455591</v>
+      </c>
       <c r="N54" s="14"/>
       <c r="O54" s="14"/>
       <c r="P54" s="14"/>
@@ -6622,6 +6754,10 @@
         <f t="shared" si="2"/>
         <v>2.159075439337804</v>
       </c>
+      <c r="M55" s="41">
+        <f t="shared" si="3"/>
+        <v>7.3584118028408394</v>
+      </c>
       <c r="N55" s="14"/>
       <c r="O55" s="14"/>
       <c r="P55" s="14"/>
@@ -6681,6 +6817,10 @@
         <f t="shared" si="2"/>
         <v>1.9799251914788032</v>
       </c>
+      <c r="M56" s="41">
+        <f t="shared" si="3"/>
+        <v>7.3953840843348697</v>
+      </c>
       <c r="N56" s="14"/>
       <c r="O56" s="14"/>
       <c r="P56" s="14"/>
@@ -6740,6 +6880,10 @@
         <f t="shared" si="2"/>
         <v>2.5425391338999681</v>
       </c>
+      <c r="M57" s="41">
+        <f t="shared" si="3"/>
+        <v>7.5817418086191504</v>
+      </c>
       <c r="N57" s="14"/>
       <c r="O57" s="14"/>
       <c r="P57" s="14"/>
@@ -6799,6 +6943,10 @@
         <f t="shared" si="2"/>
         <v>2.3184868196453503</v>
       </c>
+      <c r="M58" s="41">
+        <f t="shared" si="3"/>
+        <v>7.7020069278483501</v>
+      </c>
       <c r="N58" s="14"/>
       <c r="O58" s="14"/>
       <c r="P58" s="14"/>
@@ -6858,6 +7006,10 @@
         <f t="shared" si="2"/>
         <v>2.8956338551235925</v>
       </c>
+      <c r="M59" s="41">
+        <f t="shared" si="3"/>
+        <v>7.9137496566461802</v>
+      </c>
       <c r="N59" s="14"/>
       <c r="O59" s="14"/>
       <c r="P59" s="14"/>
@@ -6917,6 +7069,10 @@
         <f t="shared" si="2"/>
         <v>4.8443738112940755</v>
       </c>
+      <c r="M60" s="41">
+        <f t="shared" si="3"/>
+        <v>8.4528365096689093</v>
+      </c>
       <c r="N60" s="14"/>
       <c r="O60" s="14"/>
       <c r="P60" s="14"/>
@@ -6976,6 +7132,10 @@
         <f t="shared" si="2"/>
         <v>2.7976261022234121</v>
       </c>
+      <c r="M61" s="41">
+        <f t="shared" si="3"/>
+        <v>8.007830030148309</v>
+      </c>
       <c r="N61" s="14"/>
       <c r="O61" s="14"/>
       <c r="P61" s="14"/>
@@ -7035,6 +7195,10 @@
         <f t="shared" si="2"/>
         <v>2.4193864347581222</v>
       </c>
+      <c r="M62" s="41">
+        <f t="shared" si="3"/>
+        <v>8.0764149618934304</v>
+      </c>
       <c r="N62" s="14"/>
       <c r="O62" s="14"/>
       <c r="P62" s="14"/>
@@ -7094,6 +7258,10 @@
         <f t="shared" si="2"/>
         <v>2.2871355058696849</v>
       </c>
+      <c r="M63" s="41">
+        <f t="shared" si="3"/>
+        <v>8.1254077004058196</v>
+      </c>
       <c r="N63" s="14"/>
       <c r="O63" s="14"/>
       <c r="P63" s="14"/>
@@ -7153,6 +7321,10 @@
         <f t="shared" si="2"/>
         <v>1.3890541673713241</v>
       </c>
+      <c r="M64" s="41">
+        <f t="shared" si="3"/>
+        <v>8.0829607820103</v>
+      </c>
       <c r="N64" s="14"/>
       <c r="O64" s="14"/>
       <c r="P64" s="14"/>
@@ -7212,6 +7384,10 @@
         <f t="shared" si="2"/>
         <v>2.7538255433251138</v>
       </c>
+      <c r="M65" s="41">
+        <f t="shared" si="3"/>
+        <v>8.3944641523561412</v>
+      </c>
       <c r="N65" s="14"/>
       <c r="O65" s="14"/>
       <c r="P65" s="14"/>
@@ -7271,6 +7447,10 @@
         <f t="shared" si="2"/>
         <v>3.1613800715288325</v>
       </c>
+      <c r="M66" s="41">
+        <f t="shared" si="3"/>
+        <v>8.8591922776109513</v>
+      </c>
       <c r="N66" s="14"/>
       <c r="O66" s="14"/>
       <c r="P66" s="14"/>
@@ -7330,6 +7510,10 @@
         <f t="shared" si="2"/>
         <v>1.7034968365230903</v>
       </c>
+      <c r="M67" s="41">
+        <f t="shared" si="3"/>
+        <v>9.0621799214889496</v>
+      </c>
       <c r="N67" s="14"/>
       <c r="O67" s="14"/>
       <c r="P67" s="14"/>
@@ -7389,6 +7573,10 @@
         <f t="shared" si="2"/>
         <v>1.9298604312591023</v>
       </c>
+      <c r="M68" s="41">
+        <f t="shared" si="3"/>
+        <v>9.1983324528058397</v>
+      </c>
       <c r="N68" s="14"/>
       <c r="O68" s="14"/>
       <c r="P68" s="14"/>
@@ -7448,6 +7636,10 @@
         <f t="shared" si="2"/>
         <v>2.7534241143744418</v>
       </c>
+      <c r="M69" s="41">
+        <f t="shared" si="3"/>
+        <v>9.613404464707159</v>
+      </c>
       <c r="N69" s="14"/>
       <c r="O69" s="14"/>
       <c r="P69" s="14"/>
@@ -7507,6 +7699,10 @@
         <f t="shared" si="2"/>
         <v>2.1425987215016633</v>
       </c>
+      <c r="M70" s="41">
+        <f t="shared" si="3"/>
+        <v>9.6998737943510491</v>
+      </c>
       <c r="N70" s="14"/>
       <c r="O70" s="14"/>
       <c r="P70" s="14"/>
@@ -7566,6 +7762,10 @@
         <f t="shared" si="2"/>
         <v>2.1206852774365861</v>
       </c>
+      <c r="M71" s="41">
+        <f t="shared" si="3"/>
+        <v>9.8821820675085714</v>
+      </c>
       <c r="N71" s="14"/>
       <c r="O71" s="14"/>
       <c r="P71" s="14"/>
@@ -7625,6 +7825,10 @@
         <f t="shared" si="2"/>
         <v>2.6826378479932904</v>
       </c>
+      <c r="M72" s="41">
+        <f t="shared" si="3"/>
+        <v>9.8625227740041712</v>
+      </c>
       <c r="N72" s="14"/>
       <c r="O72" s="14"/>
       <c r="P72" s="14"/>
@@ -7684,6 +7888,10 @@
         <f t="shared" si="2"/>
         <v>2.3460694808167899</v>
       </c>
+      <c r="M73" s="41">
+        <f t="shared" si="3"/>
+        <v>10.268057274626351</v>
+      </c>
       <c r="N73" s="14"/>
       <c r="O73" s="14"/>
       <c r="P73" s="14"/>
@@ -7743,6 +7951,10 @@
         <f t="shared" si="2"/>
         <v>2.4766751698496057</v>
       </c>
+      <c r="M74" s="41">
+        <f t="shared" si="3"/>
+        <v>10.725870355634671</v>
+      </c>
       <c r="N74" s="14"/>
       <c r="O74" s="14"/>
       <c r="P74" s="14"/>
@@ -7802,6 +8014,10 @@
         <f t="shared" si="2"/>
         <v>1.6562763038823971</v>
       </c>
+      <c r="M75" s="41">
+        <f t="shared" si="3"/>
+        <v>10.82164709695061</v>
+      </c>
       <c r="N75" s="14"/>
       <c r="O75" s="14"/>
       <c r="P75" s="14"/>
@@ -7861,6 +8077,10 @@
         <f t="shared" si="2"/>
         <v>2.4457155101069823</v>
       </c>
+      <c r="M76" s="41">
+        <f t="shared" si="3"/>
+        <v>10.80780967241046</v>
+      </c>
       <c r="N76" s="14"/>
       <c r="O76" s="14"/>
       <c r="P76" s="14"/>
@@ -7920,6 +8140,10 @@
         <f t="shared" si="2"/>
         <v>2.4008848072742364</v>
       </c>
+      <c r="M77" s="41">
+        <f t="shared" si="3"/>
+        <v>10.94381488912085</v>
+      </c>
       <c r="N77" s="14"/>
       <c r="O77" s="14"/>
       <c r="P77" s="14"/>
@@ -7979,6 +8203,10 @@
         <f t="shared" si="2"/>
         <v>2.2593086173342507</v>
       </c>
+      <c r="M78" s="41">
+        <f t="shared" si="3"/>
+        <v>10.988895233020379</v>
+      </c>
       <c r="N78" s="14"/>
       <c r="O78" s="14"/>
       <c r="P78" s="14"/>
@@ -8038,6 +8266,10 @@
         <f t="shared" si="2"/>
         <v>1.6206271525778342</v>
       </c>
+      <c r="M79" s="41">
+        <f t="shared" si="3"/>
+        <v>10.686690452452808</v>
+      </c>
       <c r="N79" s="14"/>
       <c r="O79" s="14"/>
       <c r="P79" s="14"/>
@@ -8097,6 +8329,10 @@
         <f t="shared" si="2"/>
         <v>1.8298289115784583</v>
       </c>
+      <c r="M80" s="41">
+        <f t="shared" si="3"/>
+        <v>10.804753548957359</v>
+      </c>
       <c r="N80" s="14"/>
       <c r="O80" s="14"/>
       <c r="P80" s="14"/>
@@ -8156,6 +8392,10 @@
         <f t="shared" si="2"/>
         <v>1.80610526691359</v>
       </c>
+      <c r="M81" s="41">
+        <f t="shared" si="3"/>
+        <v>11.054497403958202</v>
+      </c>
       <c r="N81" s="14"/>
       <c r="O81" s="51"/>
       <c r="P81" s="14"/>
@@ -8215,6 +8455,10 @@
         <f t="shared" si="2"/>
         <v>1.0969134416265311</v>
       </c>
+      <c r="M82" s="41">
+        <f t="shared" si="3"/>
+        <v>11.061111782007549</v>
+      </c>
       <c r="N82" s="41"/>
       <c r="O82" s="14"/>
       <c r="P82" s="14"/>
@@ -8273,6 +8517,10 @@
       <c r="L83" s="41">
         <f t="shared" si="2"/>
         <v>0.53213412545921823</v>
+      </c>
+      <c r="M83" s="41">
+        <f t="shared" si="3"/>
+        <v>10.375887570844368</v>
       </c>
     </row>
     <row r="84" spans="1:26" ht="16.5" customHeight="1"/>

</xml_diff>